<commit_message>
Changes one name and fixation cross duration
</commit_message>
<xml_diff>
--- a/Encoding_Recall/Names_condition.xlsx
+++ b/Encoding_Recall/Names_condition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hassl\OneDrive - Lund University\Biofinder\fMRI-tasks\FacesNamesProfessions_fMRI\Encoding_Recall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7A5468-234F-4630-B0C5-7DEEAC960309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60D69AB-1FC6-4EF0-B502-84027D15B864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>Images_Faces/O48.jpg</t>
   </si>
   <si>
-    <t>Bertil</t>
-  </si>
-  <si>
     <t>Images_Faces/O49.jpg</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
   </si>
   <si>
     <t>order_randomiser</t>
+  </si>
+  <si>
+    <t>Adam</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,52 +567,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>53</v>
+        <f t="shared" ref="D2:D31" ca="1" si="0">RANDBETWEEN(1,100)</f>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>71</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>91</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,23 +626,23 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,14 +650,14 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>42</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,8 +671,8 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>23</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,8 +686,8 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -701,8 +701,8 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,8 +716,8 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>87</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -731,8 +731,8 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,23 +746,23 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>83</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,38 +776,38 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
-        <v>56</v>
-      </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>56</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>30</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -821,38 +821,38 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>67</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>98</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -866,8 +866,8 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>100</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,8 +881,8 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>42</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,8 +896,8 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>39</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,23 +911,23 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>85</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>10</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -941,8 +941,8 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>26</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,8 +956,8 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>73</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,38 +971,38 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>53</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,8 +1016,8 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>53</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>